<commit_message>
Fixed error in Total forest
</commit_message>
<xml_diff>
--- a/Table2_Terrestrial.xlsx
+++ b/Table2_Terrestrial.xlsx
@@ -437,7 +437,7 @@
         <v>6950.3281</v>
       </c>
       <c r="C2" t="n">
-        <v>-1446.1524</v>
+        <v>-208.084300000001</v>
       </c>
       <c r="D2" t="n">
         <v>3201.8016</v>
@@ -449,7 +449,7 @@
         <v>698.996</v>
       </c>
       <c r="G2" t="n">
-        <v>1867.9656</v>
+        <v>629.8975</v>
       </c>
       <c r="H2" t="n">
         <v>189.7352</v>
@@ -495,7 +495,7 @@
         <v>3878.6199</v>
       </c>
       <c r="C4" t="n">
-        <v>-932.5749</v>
+        <v>158.078100000001</v>
       </c>
       <c r="D4" t="n">
         <v>1354.244</v>
@@ -507,7 +507,7 @@
         <v>355.6422</v>
       </c>
       <c r="G4" t="n">
-        <v>1576.7815</v>
+        <v>486.1285</v>
       </c>
       <c r="H4" t="n">
         <v>159.1499</v>
@@ -524,7 +524,7 @@
         <v>1755.2911</v>
       </c>
       <c r="C5" t="n">
-        <v>-112.9524</v>
+        <v>48.2409</v>
       </c>
       <c r="D5" t="n">
         <v>900.6616</v>
@@ -536,7 +536,7 @@
         <v>323.0872</v>
       </c>
       <c r="G5" t="n">
-        <v>246.7972</v>
+        <v>85.6039</v>
       </c>
       <c r="H5" t="n">
         <v>11.3327</v>
@@ -553,7 +553,7 @@
         <v>1091.7837</v>
       </c>
       <c r="C6" t="n">
-        <v>-212.6432</v>
+        <v>11.4981</v>
       </c>
       <c r="D6" t="n">
         <v>503.8269</v>
@@ -565,7 +565,7 @@
         <v>100.4372</v>
       </c>
       <c r="G6" t="n">
-        <v>360.0377</v>
+        <v>135.8964</v>
       </c>
       <c r="H6" t="n">
         <v>43.1797</v>
@@ -611,7 +611,7 @@
         <v>439.6053</v>
       </c>
       <c r="C8" t="n">
-        <v>-35.3267</v>
+        <v>80.7752</v>
       </c>
       <c r="D8" t="n">
         <v>221.342</v>
@@ -623,7 +623,7 @@
         <v>71.2681</v>
       </c>
       <c r="G8" t="n">
-        <v>120.2188</v>
+        <v>4.1169</v>
       </c>
       <c r="H8" t="n">
         <v>8.019</v>
@@ -640,7 +640,7 @@
         <v>255.3549</v>
       </c>
       <c r="C9" t="n">
-        <v>-7.19880000000001</v>
+        <v>1.69289999999995</v>
       </c>
       <c r="D9" t="n">
         <v>80.4886</v>
@@ -652,7 +652,7 @@
         <v>6.1841</v>
       </c>
       <c r="G9" t="n">
-        <v>98.9771</v>
+        <v>90.0854</v>
       </c>
       <c r="H9" t="n">
         <v>8.6781</v>
@@ -669,7 +669,7 @@
         <v>227.5754</v>
       </c>
       <c r="C10" t="n">
-        <v>-79.9205</v>
+        <v>-56.5546</v>
       </c>
       <c r="D10" t="n">
         <v>110.1405</v>
@@ -681,7 +681,7 @@
         <v>50.5277</v>
       </c>
       <c r="G10" t="n">
-        <v>48.3676</v>
+        <v>25.0017</v>
       </c>
       <c r="H10" t="n">
         <v>7.2627</v>
@@ -698,7 +698,7 @@
         <v>56.735</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.6737</v>
+        <v>3.5311</v>
       </c>
       <c r="D11" t="n">
         <v>4.2924</v>
@@ -710,7 +710,7 @@
         <v>0.3062</v>
       </c>
       <c r="G11" t="n">
-        <v>22.3098</v>
+        <v>17.105</v>
       </c>
       <c r="H11" t="n">
         <v>1.6063</v>

</xml_diff>